<commit_message>
Update-MC Inv Home VIII
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/Inventory-ReportTemplate.xlsx
+++ b/bin/Debug/Template/Inventory-ReportTemplate.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Project\My C# project\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4663FAF2-CB4E-4358-B191-E82C56B42236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7F5A3F-11ED-49EA-8EE8-A153DEA43A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{7A6E4813-BD53-49E0-9004-164D632BEFC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{7A6E4813-BD53-49E0-9004-164D632BEFC8}"/>
   </bookViews>
   <sheets>
     <sheet name="KIT" sheetId="2" r:id="rId1"/>
     <sheet name="SD" sheetId="3" r:id="rId2"/>
-    <sheet name="Inprocess" sheetId="1" r:id="rId3"/>
+    <sheet name="Inprocess-POS" sheetId="5" r:id="rId3"/>
+    <sheet name="Inprocess-Semi" sheetId="4" r:id="rId4"/>
+    <sheet name="Inprocess-SD" sheetId="6" r:id="rId5"/>
+    <sheet name="Inprocess-NG" sheetId="7" r:id="rId6"/>
+    <sheet name="Inprocess" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Inprocess!$A$7:$F$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Inprocess!$A$7:$F$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Inprocess-NG'!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Inprocess-POS'!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Inprocess-SD'!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Inprocess-Semi'!$A$1:$I$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="6">Inprocess!$7:$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t xml:space="preserve">RM Code </t>
   </si>
@@ -95,12 +104,45 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>RM Code</t>
+  </si>
+  <si>
+    <t>RM Name</t>
+  </si>
+  <si>
+    <t>Document No</t>
+  </si>
+  <si>
+    <t>POS No</t>
+  </si>
+  <si>
+    <t>WIP Qty</t>
+  </si>
+  <si>
+    <t>WIP Name</t>
+  </si>
+  <si>
+    <t>Label No</t>
+  </si>
+  <si>
+    <t>Usage Qty</t>
+  </si>
+  <si>
+    <t>MCSeq No</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0000"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +191,21 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -211,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -227,6 +284,54 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -234,7 +339,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFC000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1565,14 +1692,254 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E888930D-F0DF-48C6-A83C-7C2373B99599}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="10"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F2" xr:uid="{E888930D-F0DF-48C6-A83C-7C2373B99599}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A4BCC8-E404-4C05-962A-A4D2CE6A69E3}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="19"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I2" xr:uid="{96A4BCC8-E404-4C05-962A-A4D2CE6A69E3}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46E70EC-3C3E-4DAF-81ED-A46209201784}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="15"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F2" xr:uid="{B46E70EC-3C3E-4DAF-81ED-A46209201784}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1365C9-FF39-4E60-B1FE-EF64AF799796}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="23"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F2" xr:uid="{6D1365C9-FF39-4E60-B1FE-EF64AF799796}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771DB528-ABEE-4DB8-96C1-6F19C2D53566}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,14 +1955,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1635,7 +2002,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
@@ -1647,8 +2014,22 @@
   <mergeCells count="1">
     <mergeCell ref="A2:F2"/>
   </mergeCells>
-  <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.2" header="0.3" footer="0.08"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>

</xml_diff>